<commit_message>
Updated SAU model - 2025-08-21 12:21
</commit_message>
<xml_diff>
--- a/VerveStacks_SAU/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_SAU/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_SAU\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{94E9879B-EB7B-44B7-B23D-E679B2582EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{47A06D24-85E9-4E5D-B46D-9E77CB14E5B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1827,7 +1827,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36D4B316-F1BE-A25C-4500-0CD7214F5F72}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AE5EFDC-6328-65DE-7797-2B5A48B90BEE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1882,7 +1882,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8203615C-E66D-74C0-CEED-BA40F07E6E2A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E8B5080-0D67-1BC5-9E03-BA4A2F797AC6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1937,7 +1937,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE5D00BC-EFB6-80E1-EE96-82FA8756B76C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F27F316-B62D-5E89-E40E-8658E8A5E6D4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1992,7 +1992,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{207BC572-EDFF-200C-6CFB-ABEB45194002}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89199E08-9471-370F-1A92-B4454A26D63D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4413,7 +4413,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C508DF1-1EB9-457A-BCB2-C7D2A98D0E43}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CDD6C31-076C-4870-93DE-FD6C2B895B3C}">
   <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5572,7 +5572,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9D0A6CB-9741-4CC1-9960-D0E868A2F2AC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46BB8B48-1EA4-4718-AB7C-F80130B1B489}">
   <dimension ref="A1:P124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10626,7 +10626,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBA931CD-4BA2-482B-BCF2-C4BAC21FAD8C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F911EA8F-2A59-481B-B54D-1126DC144A23}">
   <dimension ref="A1:Q57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated SAU model - 2025-08-21 22:57
</commit_message>
<xml_diff>
--- a/VerveStacks_SAU/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_SAU/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_SAU\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5302DB67-E50D-4D1D-974F-2599B03F0DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{26E26C9F-5B53-4ED2-9829-97E2C01CD8A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="2205" windowWidth="21600" windowHeight="12683" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="misc" sheetId="7" r:id="rId1"/>
@@ -862,16 +862,16 @@
     <t>wind resource -- CF class won-SAU_37 -- cost class 1</t>
   </si>
   <si>
+    <t>e_won-SAU_36_c5</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-SAU_36 -- cost class 5</t>
+  </si>
+  <si>
     <t>e_won-SAU_36_c4</t>
   </si>
   <si>
     <t>wind resource -- CF class won-SAU_36 -- cost class 4</t>
-  </si>
-  <si>
-    <t>e_won-SAU_36_c5</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-SAU_36 -- cost class 5</t>
   </si>
   <si>
     <t>e_won-SAU_36_c3</t>
@@ -2641,7 +2641,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D05DA397-761A-9204-74F0-31887559D083}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{554446FE-C34A-71CB-8FB4-6780EA9F3D85}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2696,7 +2696,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA1569DE-51E2-D30C-CAC0-B162B91AAC69}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F06ED951-8BD0-809F-A7B0-59A3A91ED4BE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2751,7 +2751,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43A50BCD-F69A-1D1F-11C3-B5896B1C7DE8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14378B7E-253C-992C-A1D2-32B7CCAD98EF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2806,7 +2806,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1937B397-C0E7-DE5D-E20E-B6A2F69A46B1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A1EF526-5EDD-9944-5A2F-84274143DB33}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6630,7 +6630,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5378AA5E-20FE-48F4-B7F5-9A22906535F3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0382C47A-C1BA-4408-8CA5-33F99D1D9265}">
   <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7789,7 +7789,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5730FC22-2DE7-481D-82A0-315BBA709C32}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE447303-2030-4D8D-8F65-FF9BB0BFAA52}">
   <dimension ref="A1:P124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8270,16 +8270,16 @@
         <v>468</v>
       </c>
       <c r="M13" s="161">
-        <v>11.61</v>
+        <v>5.78775</v>
       </c>
       <c r="N13" s="162">
         <v>0.36199999999999999</v>
       </c>
       <c r="O13" s="161">
-        <v>31.110414183102254</v>
+        <v>39.685731787457968</v>
       </c>
       <c r="P13" s="163">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -8311,16 +8311,16 @@
         <v>468</v>
       </c>
       <c r="M14" s="158">
-        <v>5.78775</v>
+        <v>11.61</v>
       </c>
       <c r="N14" s="159">
         <v>0.36199999999999999</v>
       </c>
       <c r="O14" s="158">
-        <v>39.685731787457968</v>
+        <v>31.110414183102254</v>
       </c>
       <c r="P14" s="160">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -12843,7 +12843,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6249B8C-0B61-46EE-BAAF-D1225867FEE4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E333F1-6CE3-42F2-BE5A-BEA41B2BF86E}">
   <dimension ref="A1:Q57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated SAU model - 2025-08-21 23:02
</commit_message>
<xml_diff>
--- a/VerveStacks_SAU/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_SAU/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_SAU\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{26E26C9F-5B53-4ED2-9829-97E2C01CD8A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A19C72A2-F8E0-4B9F-BD42-2D0D65F4A303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -826,18 +826,18 @@
     <t>wind resource -- CF class won-SAU_40 -- cost class 1</t>
   </si>
   <si>
+    <t>e_won-SAU_38_c1</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-SAU_38 -- cost class 1</t>
+  </si>
+  <si>
     <t>e_won-SAU_38_c2</t>
   </si>
   <si>
     <t>wind resource -- CF class won-SAU_38 -- cost class 2</t>
   </si>
   <si>
-    <t>e_won-SAU_38_c1</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-SAU_38 -- cost class 1</t>
-  </si>
-  <si>
     <t>e_won-SAU_38_c3</t>
   </si>
   <si>
@@ -862,16 +862,16 @@
     <t>wind resource -- CF class won-SAU_37 -- cost class 1</t>
   </si>
   <si>
+    <t>e_won-SAU_36_c4</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-SAU_36 -- cost class 4</t>
+  </si>
+  <si>
     <t>e_won-SAU_36_c5</t>
   </si>
   <si>
     <t>wind resource -- CF class won-SAU_36 -- cost class 5</t>
-  </si>
-  <si>
-    <t>e_won-SAU_36_c4</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-SAU_36 -- cost class 4</t>
   </si>
   <si>
     <t>e_won-SAU_36_c3</t>
@@ -2641,7 +2641,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{554446FE-C34A-71CB-8FB4-6780EA9F3D85}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F8B63D4-C8DB-E794-B2A6-6ADFB7A852D3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2696,7 +2696,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F06ED951-8BD0-809F-A7B0-59A3A91ED4BE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFB6A193-C785-4F33-4E7C-CBFFE00E2D7D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2751,7 +2751,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14378B7E-253C-992C-A1D2-32B7CCAD98EF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65A7F1C9-17C8-B6C2-D320-B583C0B0F7A1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2806,7 +2806,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A1EF526-5EDD-9944-5A2F-84274143DB33}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8B093F9-4A5D-908F-0C4B-44D1A3464A2A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6630,7 +6630,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0382C47A-C1BA-4408-8CA5-33F99D1D9265}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{518FBD16-FB3B-4C1E-BEDF-EBE8FB2C8EDC}">
   <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7789,7 +7789,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE447303-2030-4D8D-8F65-FF9BB0BFAA52}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A9130FC-3DDA-44A0-916B-883C7C7661AB}">
   <dimension ref="A1:P124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8024,16 +8024,16 @@
         <v>468</v>
       </c>
       <c r="M7" s="161">
-        <v>5.6047500000000001</v>
+        <v>5.5642500000000004</v>
       </c>
       <c r="N7" s="162">
         <v>0.38099999999999995</v>
       </c>
       <c r="O7" s="161">
-        <v>24.31630123130919</v>
+        <v>23.86258072314212</v>
       </c>
       <c r="P7" s="163">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -8065,16 +8065,16 @@
         <v>468</v>
       </c>
       <c r="M8" s="158">
-        <v>5.5642500000000004</v>
+        <v>5.6047500000000001</v>
       </c>
       <c r="N8" s="159">
         <v>0.38099999999999995</v>
       </c>
       <c r="O8" s="158">
-        <v>23.86258072314212</v>
+        <v>24.31630123130919</v>
       </c>
       <c r="P8" s="160">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -8270,16 +8270,16 @@
         <v>468</v>
       </c>
       <c r="M13" s="161">
-        <v>5.78775</v>
+        <v>11.61</v>
       </c>
       <c r="N13" s="162">
         <v>0.36199999999999999</v>
       </c>
       <c r="O13" s="161">
-        <v>39.685731787457968</v>
+        <v>31.110414183102254</v>
       </c>
       <c r="P13" s="163">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -8311,16 +8311,16 @@
         <v>468</v>
       </c>
       <c r="M14" s="158">
-        <v>11.61</v>
+        <v>5.78775</v>
       </c>
       <c r="N14" s="159">
         <v>0.36199999999999999</v>
       </c>
       <c r="O14" s="158">
-        <v>31.110414183102254</v>
+        <v>39.685731787457968</v>
       </c>
       <c r="P14" s="160">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -12843,7 +12843,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E333F1-6CE3-42F2-BE5A-BEA41B2BF86E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD9CF9D6-9994-47AE-9D91-5F550A426DB5}">
   <dimension ref="A1:Q57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>